<commit_message>
Se modificó nombre del archivo generado
</commit_message>
<xml_diff>
--- a/ComparadorWebform/Archivos/Output/ArchivoComparacionExcel.xlsx
+++ b/ComparadorWebform/Archivos/Output/ArchivoComparacionExcel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <x:si>
     <x:t>COMPARACIÓN DE ARCHIVOS</x:t>
   </x:si>
@@ -35,25 +35,37 @@
     <x:t>IMPORTE</x:t>
   </x:si>
   <x:si>
-    <x:t>PAGO BOSTON SEG 00867510</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DEBITO TRANSF CONNECTION BANKING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRANSF. E/BCOS-ONLINE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7000,13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DEP.EFVO.TJ 589244501500000002</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PAGO FED PATRON 71000000100121</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CREDITO INMEDIATO</x:t>
+    <x:t xml:space="preserve">Transferencia Realizada  - A Barrera, Mariano Dan /varios -var/20206476738 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pago De Servicios  - Aysa: 0003550606 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pago De Haberes  - 00720014007003751882ars </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pago A Proveedores Recibido  - Combril Sa 33712043089 03 2618248 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pago A Proveedores Recibido  - Combril Sa 33712043089 03 2609006 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Debito Automatico  - Fed Patronal Sa -1800538472000000101220 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pago A Proveedores Recibido  - Combril Sa 33712043089 03 2619608 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Debito Transf. Online Banking Emp  - A Boston Compania Arg De Seg Sa/seguro -seg/30500001115 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Snp Debito Directo  - Metrogas Sa -030004626471 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Transferencia Realizada  - A Cbu 0340100808710151112007 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Debito Automatico  - Edenor -005877975753 </x:t>
   </x:si>
   <x:si>
     <x:t>Conceptos presentes en Octoupus y no en Banco</x:t>
@@ -65,34 +77,61 @@
     <x:t>HABER</x:t>
   </x:si>
   <x:si>
-    <x:t>Pago Expensas N° UF 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEGURO INTEGRAL DEL CONSORCIO - PÓLIZA 33777 - CUOTA 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SUELDO DIDEK, IVAN ALEXANDER - 12/2020</x:t>
+    <x:t>BANCO RIO - CTA. CTE. N° 014-011865-1 IMPUESTO A LOS DEBITOS Y CRÉDITOS - (Período Diciembre)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANCO RIO - CTA. CTE. N° 014-011865-1 GASTOS DE MANTENIMIENTO - (Período Diciembre)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SERVICIO DE ADMINISTRACIÓN DE COBRANZAS ELECTRONICAS - (Período Diciembre)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PARRILLA TERRAZA:DESARME Y RETIRO DE ESCOMBROS PARA LAS INSTALACIÓN DE LA NUEVA PARRILLA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7B POR FILTRACIONES SE REALIZA ESCALON DE CEMNETO RECTO REVISTIÉNDOSE CON CERÁMICAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PIEDRA 20 BA MAVO-ARENA 20DM3- ARC REFRACK 10K- REJA BARRA RED-CAL COM 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CUENTA N° 3550606 - CONSUMO 350 M3 - PERÍODO 13/11/2020 AL 13/12/2020 FACT 0108B66608456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CUENTA N° 3550606 - CONSUMO 350 M3 - PERÍODO 13/11/2020 AL 13/12/2020 - COCHERA - FACT 0108B66608456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SUELDO KURIS, BERNARDO - 12/2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CUENTA N° 3550606 - CONSUMO 350 M3 PERÍODO 13/11/2020 AL 13/12/2020 FACT- 0108B66608456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CUENTA N° 3550606 - CONSUMO 350 M3 PERÍODO 13/11/2020 AL 13/12/2020 FACT- 0108B66608456 - COCHERA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FOTOCOPIAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diciembre 2020 - Pago Mi Expensa</x:t>
   </x:si>
   <x:si>
     <x:t>Sumatoria Códigos Excluidos Banco:</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Sumatoria código 259 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sumatoria código 260 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sumatoria código 212 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sumatoria código 207 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sumatoria código 206 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sumatoria código 515 </x:t>
+    <x:t xml:space="preserve">Sumatoria código 4633 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sumatoria código 4637 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sumatoria código 3254 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sumatoria código 1924 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sumatoria código 2960 </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">TOTAL CODIGOS EXCLUIDOS </x:t>
@@ -454,7 +493,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E29"/>
+  <x:dimension ref="A1:E43"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -486,264 +525,466 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="1">
-        <x:v>44215</x:v>
+        <x:v>44187</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
-        <x:v>858</x:v>
+        <x:v>824</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>-2840</x:v>
+        <x:v>-13700</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="1">
-        <x:v>44215</x:v>
+        <x:v>44187</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
-        <x:v>990</x:v>
+        <x:v>4719</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>-8100</x:v>
+        <x:v>-20023.83</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="1">
-        <x:v>44215</x:v>
+        <x:v>44186</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
-        <x:v>783</x:v>
+        <x:v>2676</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>9</x:v>
+      <x:c r="D7" s="0" t="n">
+        <x:v>-38678</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="1">
-        <x:v>44210</x:v>
+        <x:v>44186</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
-        <x:v>399</x:v>
+        <x:v>4719</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>-20370.72</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="1">
-        <x:v>44210</x:v>
+        <x:v>44181</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
-        <x:v>399</x:v>
+        <x:v>2377</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>22945.76</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="1">
-        <x:v>44210</x:v>
+        <x:v>44180</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
-        <x:v>399</x:v>
+        <x:v>2377</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
-        <x:v>500</x:v>
+        <x:v>14425.72</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="1">
-        <x:v>44210</x:v>
+        <x:v>44179</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
-        <x:v>399</x:v>
+        <x:v>4085</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
-        <x:v>7000</x:v>
+        <x:v>-792</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="1">
-        <x:v>44208</x:v>
+        <x:v>44176</x:v>
       </x:c>
       <x:c r="B12" s="0" t="n">
-        <x:v>858</x:v>
+        <x:v>2377</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
-        <x:v>-210</x:v>
+        <x:v>8833.43</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="1">
-        <x:v>44207</x:v>
+        <x:v>44175</x:v>
       </x:c>
       <x:c r="B13" s="0" t="n">
-        <x:v>785</x:v>
+        <x:v>1252</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D13" s="0" t="n">
-        <x:v>6314</x:v>
+        <x:v>-3850</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="1">
-        <x:v>44203</x:v>
+        <x:v>44160</x:v>
       </x:c>
       <x:c r="B14" s="0" t="n">
-        <x:v>990</x:v>
+        <x:v>4081</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D14" s="0" t="n">
-        <x:v>-4678</x:v>
+        <x:v>-741.26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5">
+      <x:c r="A15" s="1">
+        <x:v>44159</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>824</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="n">
+        <x:v>-710</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
-      <x:c r="A16" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5">
-      <x:c r="A17" s="0" t="s">
+      <x:c r="A16" s="1">
+        <x:v>44159</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>4085</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="n">
+        <x:v>-1049.57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5">
+      <x:c r="A18" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="A19" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
+      <x:c r="C19" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="A18" s="1">
-        <x:v>44211</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="n">
-        <x:v>7700</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5">
-      <x:c r="A19" s="1">
-        <x:v>44211</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="n">
-        <x:v>-2119</x:v>
+      <x:c r="D19" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="1">
-        <x:v>44202</x:v>
+        <x:v>44188</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>-4677</x:v>
+        <x:v>-2582.45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="A21" s="1">
+        <x:v>44188</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="n">
+        <x:v>-1397</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
-      <x:c r="A22" s="0" t="s">
-        <x:v>19</x:v>
+      <x:c r="A22" s="1">
+        <x:v>44188</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="n">
+        <x:v>-1740.42</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
-      <x:c r="A23" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="n">
-        <x:v>-906.41</x:v>
+      <x:c r="A23" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="n">
+        <x:v>-4500</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
-      <x:c r="A24" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="n">
-        <x:v>-634.98</x:v>
+      <x:c r="A24" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="n">
+        <x:v>-10500</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
-      <x:c r="A25" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="n">
-        <x:v>-130.8</x:v>
+      <x:c r="A25" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="n">
+        <x:v>2731</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
-      <x:c r="A26" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="n">
-        <x:v>-276.86</x:v>
+      <x:c r="A26" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="n">
+        <x:v>-19210.3</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
-      <x:c r="A27" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="n">
-        <x:v>-457.8</x:v>
+      <x:c r="A27" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="n">
+        <x:v>-1160.42</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
-      <x:c r="A28" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="n">
-        <x:v>-2180</x:v>
+      <x:c r="A28" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="n">
+        <x:v>-7805</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
-      <x:c r="A29" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="n">
-        <x:v>-4586.85</x:v>
+      <x:c r="A29" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="n">
+        <x:v>-30872</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:5">
+      <x:c r="A30" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="n">
+        <x:v>-18863.41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:5">
+      <x:c r="A31" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="n">
+        <x:v>-1160.42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:5">
+      <x:c r="A32" s="1">
+        <x:v>44186</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="n">
+        <x:v>-106</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:5">
+      <x:c r="A33" s="1">
+        <x:v>44175</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="n">
+        <x:v>23810.07</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:5">
+      <x:c r="A34" s="1">
+        <x:v>44174</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="n">
+        <x:v>14969.1</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:5">
+      <x:c r="A35" s="1">
+        <x:v>44168</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="n">
+        <x:v>9166.16</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:5">
+      <x:c r="A37" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:5">
+      <x:c r="A38" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="n">
+        <x:v>-1533.81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:5">
+      <x:c r="A39" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="n">
+        <x:v>-1099.89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:5">
+      <x:c r="A40" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="n">
+        <x:v>-231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:5">
+      <x:c r="A41" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="n">
+        <x:v>-66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:5">
+      <x:c r="A42" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="n">
+        <x:v>-1100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:5">
+      <x:c r="A43" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="n">
+        <x:v>-4030.7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>